<commit_message>
deepika - 24th May
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/AutomationTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/AutomationTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deepika\Sunrun\crmautomation\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742B34EF-E7AB-4C04-AF43-D809F65A77D2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0CC2B4-A135-4C82-93E5-1C4113E5742D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Leads" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
   <si>
     <t>Bulk Mail</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>D2H_LeadD@yopmail.com</t>
-  </si>
-  <si>
-    <t>Visibility</t>
   </si>
 </sst>
 </file>
@@ -648,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8605BC2E-416F-42B3-84A2-B10816354C93}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -903,10 +900,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AD8BD9-3163-4ED5-AF75-487BD02048D4}">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -916,7 +913,7 @@
     <col min="3" max="3" width="39.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -926,11 +923,8 @@
       <c r="C1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -940,38 +934,35 @@
       <c r="C2" t="s">
         <v>58</v>
       </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" t="s">
+        <v>57</v>
+      </c>
       <c r="C3" t="s">
         <v>45</v>
       </c>
-      <c r="D3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="3"/>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
       <c r="C4" t="s">
         <v>46</v>
       </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="3"/>
+      <c r="B5" t="s">
+        <v>57</v>
+      </c>
       <c r="C5" t="s">
         <v>53</v>
       </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -981,38 +972,35 @@
       <c r="C6" t="s">
         <v>58</v>
       </c>
-      <c r="D6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
+      <c r="B7" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" t="s">
         <v>45</v>
       </c>
-      <c r="D7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
+      <c r="B8" t="s">
+        <v>43</v>
+      </c>
       <c r="C8" t="s">
         <v>46</v>
       </c>
-      <c r="D8" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
+      <c r="B9" t="s">
+        <v>43</v>
+      </c>
       <c r="C9" t="s">
         <v>53</v>
       </c>
-      <c r="D9" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>42</v>
       </c>
@@ -1022,36 +1010,35 @@
       <c r="C10" t="s">
         <v>58</v>
       </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" s="3"/>
+      <c r="B11" t="s">
+        <v>43</v>
+      </c>
       <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="D11" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="3"/>
+      <c r="B12" t="s">
+        <v>43</v>
+      </c>
       <c r="C12" t="s">
         <v>46</v>
       </c>
-      <c r="D12" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="3"/>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
       <c r="C13" t="s">
         <v>53</v>
       </c>
-      <c r="D13" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
         <v>51</v>
       </c>
@@ -1061,32 +1048,32 @@
       <c r="C14" t="s">
         <v>58</v>
       </c>
-      <c r="D14" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="3"/>
+      <c r="B15" t="s">
+        <v>52</v>
+      </c>
       <c r="C15" t="s">
         <v>45</v>
       </c>
-      <c r="D15" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="3"/>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
       <c r="C16" t="s">
         <v>46</v>
       </c>
-      <c r="D16" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3"/>
+      <c r="B17" t="s">
+        <v>52</v>
+      </c>
       <c r="C17" t="s">
         <v>53</v>
-      </c>
-      <c r="D17" t="b">
-        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
deepika - 3rd Dec,2021
</commit_message>
<xml_diff>
--- a/src/main/java/com/crm/qa/testdata/AutomationTestData.xlsx
+++ b/src/main/java/com/crm/qa/testdata/AutomationTestData.xlsx
@@ -1,23 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Deepika\Sunrun\crmautomation\src\main\java\com\crm\qa\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB0CC2B4-A135-4C82-93E5-1C4113E5742D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E49671A0-4191-46D2-84C6-B1A41FF2097A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Leads" sheetId="1" r:id="rId1"/>
-    <sheet name="D2HLeadCreation" sheetId="2" r:id="rId2"/>
-    <sheet name="D2HLeadSearch" sheetId="3" r:id="rId3"/>
+    <sheet name="ResidentialAccount" sheetId="5" r:id="rId1"/>
+    <sheet name="Opportunity" sheetId="6" r:id="rId2"/>
+    <sheet name="Contacts" sheetId="4" r:id="rId3"/>
+    <sheet name="Leads" sheetId="1" r:id="rId4"/>
+    <sheet name="D2HLeadCreation" sheetId="2" r:id="rId5"/>
+    <sheet name="D2HLeadSearch" sheetId="3" r:id="rId6"/>
+    <sheet name="LeadAPIData" sheetId="8" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="150">
   <si>
     <t>Bulk Mail</t>
   </si>
@@ -210,6 +214,333 @@
   </si>
   <si>
     <t>D2H_LeadD@yopmail.com</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>LName</t>
+  </si>
+  <si>
+    <t>AccName</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>CallCon</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>LeadSource</t>
+  </si>
+  <si>
+    <t>PrefConMethod</t>
+  </si>
+  <si>
+    <t>MySunCustID</t>
+  </si>
+  <si>
+    <t>MailingStreet</t>
+  </si>
+  <si>
+    <t>MailingCity</t>
+  </si>
+  <si>
+    <t>MailingState</t>
+  </si>
+  <si>
+    <t>MailingZip</t>
+  </si>
+  <si>
+    <t>MailingCountry</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>AddressStaStatus</t>
+  </si>
+  <si>
+    <t>CreditSubmitted</t>
+  </si>
+  <si>
+    <t>CreditReceived</t>
+  </si>
+  <si>
+    <t>27370 Silent Water Way-89149</t>
+  </si>
+  <si>
+    <t>(256) 283-3633</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>DemoKathy.Reaves@yopmail.com</t>
+  </si>
+  <si>
+    <t>LGCY</t>
+  </si>
+  <si>
+    <t>7370 Silent Water Way</t>
+  </si>
+  <si>
+    <t>Las Vegas</t>
+  </si>
+  <si>
+    <t>NV</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Standardization Required</t>
+  </si>
+  <si>
+    <t>7/22/2021 2:02 AM</t>
+  </si>
+  <si>
+    <t>Incorporated</t>
+  </si>
+  <si>
+    <t>AddressStandardizationStatus</t>
+  </si>
+  <si>
+    <t>AddressStandardizationSource</t>
+  </si>
+  <si>
+    <t>AddressToken</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>AddStaConfiLevel</t>
+  </si>
+  <si>
+    <t>TimeZone</t>
+  </si>
+  <si>
+    <t>HasDaylightSavings</t>
+  </si>
+  <si>
+    <t>AreaCode</t>
+  </si>
+  <si>
+    <t>CongressDistrictNumber</t>
+  </si>
+  <si>
+    <t>StateLegislativeUpper</t>
+  </si>
+  <si>
+    <t>StateLegislativeLower</t>
+  </si>
+  <si>
+    <t>Standardized</t>
+  </si>
+  <si>
+    <t>Google Maps</t>
+  </si>
+  <si>
+    <t>USA:NV:LAS VEGAS:SILENT WATER WAY:7370:89149</t>
+  </si>
+  <si>
+    <t>ROOFTOP</t>
+  </si>
+  <si>
+    <t>PST</t>
+  </si>
+  <si>
+    <t>AutomationTestAccount</t>
+  </si>
+  <si>
+    <t>SiteDesignReqDate</t>
+  </si>
+  <si>
+    <t>SalesRepEmail</t>
+  </si>
+  <si>
+    <t>SalesBranch</t>
+  </si>
+  <si>
+    <t>SalesTerritory</t>
+  </si>
+  <si>
+    <t>LeadOrigin</t>
+  </si>
+  <si>
+    <t>RackingType</t>
+  </si>
+  <si>
+    <t>Program</t>
+  </si>
+  <si>
+    <t>HOAPhone</t>
+  </si>
+  <si>
+    <t>DialStatus</t>
+  </si>
+  <si>
+    <t>ProductOffering</t>
+  </si>
+  <si>
+    <t>Channel</t>
+  </si>
+  <si>
+    <t>LeadType</t>
+  </si>
+  <si>
+    <t>Stage</t>
+  </si>
+  <si>
+    <t>CloseDate</t>
+  </si>
+  <si>
+    <t>Probability</t>
+  </si>
+  <si>
+    <t>OpportunityNumber</t>
+  </si>
+  <si>
+    <t>ChannelLast</t>
+  </si>
+  <si>
+    <t>LeadSourceLast</t>
+  </si>
+  <si>
+    <t>LeadTypeLast</t>
+  </si>
+  <si>
+    <t>TechnologyLast</t>
+  </si>
+  <si>
+    <t>DealRegistrationStatus</t>
+  </si>
+  <si>
+    <t>7/31/2019 1:50 PM</t>
+  </si>
+  <si>
+    <t>raymond.abati@sunrun.com.invalid</t>
+  </si>
+  <si>
+    <t>Las Vegas1</t>
+  </si>
+  <si>
+    <t>SunRun</t>
+  </si>
+  <si>
+    <t>SNR UR TR</t>
+  </si>
+  <si>
+    <t>BP 1</t>
+  </si>
+  <si>
+    <t>(702) 448-8118</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Solar + Storage</t>
+  </si>
+  <si>
+    <t>Sales Partner</t>
+  </si>
+  <si>
+    <t>Partner</t>
+  </si>
+  <si>
+    <t>7. Closed Won</t>
+  </si>
+  <si>
+    <t>O-1885107440</t>
+  </si>
+  <si>
+    <t>BrightPath Mobile</t>
+  </si>
+  <si>
+    <t>New Deal</t>
+  </si>
+  <si>
+    <t>Kathy</t>
+  </si>
+  <si>
+    <t>Reaves</t>
+  </si>
+  <si>
+    <t>ReqBody</t>
+  </si>
+  <si>
+    <t>{"customerFirstName":"XT",
+"customerLastName":"XT",
+"customerStreet":"32812 S Folklore Loop",
+"customerFullAddress":"32812 S Folklore Loop, Union City, CA 94587",
+"janUsage":"900",
+"febUsage":"900",
+"marUsage":"900",
+"aprUsage":"900",
+"mayUsage":"900",
+"junUsage":"900",
+"julUsage":"900",
+"augUsage":"900",
+"sepUsage":"900",
+"octUsage":"900",
+"novUsage":"900",
+"decUsage":"900",
+"accountNumber":"",
+"additionalServices":"Energy Storage / Bright Box Battery;",
+"averageMonthlyElectricBill":"$351-400",
+"channel":"Self Gen",
+"customerCity":"Union City",
+"customerEmail":"sunrun@yopmail.com",
+"customerPrimaryPhone":"(801) 354-6513",
+"customerState":"CA",
+"customerZipCode":"94587",
+"hasHoa":"No",
+"homeSize":"",
+"homeType":"Detached single family home",
+"latitude":38.554088,"leadSource":"Sales Self Gen",
+"leadStage":"",
+"leadStatus":"",
+"longitude":-121.4654132,
+"memberId":"",
+"memberType":"",
+"meterNumber":"",
+"mobilePhone":"(801) 354-6513",
+"notes":"",
+"preferredLanguage":"English",
+"preferredLanguageContact":"",
+"purchasedThru":"Standard (Non-Retail)",
+"reason":"",
+"rentorOwn":"Own",
+"retailStoreLocation":"",
+"roofingType":"Comp Shingle",
+"sunrunCallConsent":"Yes",
+"utilityBillDate":"",
+"utilityServiceAddress":"",
+"costcoType":"",
+"isAnnualUsageAvailable":true,
+"utilityCompany":"PG&amp;E",
+"rateSchedule":"E-1",
+"leadType":"Rep Self Gen",
+"externalSource":"Sales Platform",
+"leadRep":"00552000005ezjc",
+"cityName":"Union City",
+"cityType":"City",
+"countyName":"CA",
+"incorporationFlag":"yes","townshipName":"Union City",
+"dncCoreLogicApi":true,
+"coreLogicC2DStatus":"Failure",
+"coreLogicSpatialStatus":"Success"}</t>
   </si>
 </sst>
 </file>
@@ -241,12 +572,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -262,11 +599,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -547,6 +891,479 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0F343C5-50D7-4CE9-BE49-53D5BE56D7D5}">
+  <dimension ref="A1:AH2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.77734375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="25.44140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="24" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="10.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:34" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
+      <c r="AD1" s="6"/>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
+      <c r="AG1" s="5"/>
+      <c r="AH1" s="5"/>
+    </row>
+    <row r="2" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F2">
+        <v>36.295095400000001</v>
+      </c>
+      <c r="G2">
+        <v>-115.3072331</v>
+      </c>
+      <c r="H2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I2" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>702</v>
+      </c>
+      <c r="L2">
+        <v>4</v>
+      </c>
+      <c r="M2">
+        <v>18</v>
+      </c>
+      <c r="N2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49D5DEFF-7A02-46CA-9FCC-073F2F00739B}">
+  <dimension ref="A1:V2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="16.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D2" t="s">
+        <v>133</v>
+      </c>
+      <c r="E2" t="s">
+        <v>134</v>
+      </c>
+      <c r="F2" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" t="s">
+        <v>136</v>
+      </c>
+      <c r="H2" t="s">
+        <v>137</v>
+      </c>
+      <c r="I2" t="s">
+        <v>138</v>
+      </c>
+      <c r="J2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K2" t="s">
+        <v>140</v>
+      </c>
+      <c r="L2" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" t="s">
+        <v>142</v>
+      </c>
+      <c r="O2" s="7">
+        <v>43593</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>143</v>
+      </c>
+      <c r="R2" t="s">
+        <v>140</v>
+      </c>
+      <c r="S2" t="s">
+        <v>84</v>
+      </c>
+      <c r="T2" t="s">
+        <v>141</v>
+      </c>
+      <c r="U2" t="s">
+        <v>144</v>
+      </c>
+      <c r="V2" t="s">
+        <v>145</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F9EEB44D-5E92-406D-A832-14CBBFD1D544}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE656C60-29FD-46ED-BFC3-FFD250CA1F72}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.21875" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" t="s">
+        <v>147</v>
+      </c>
+      <c r="C2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D2" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2">
+        <v>8.7973605382625403E+18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L2" t="s">
+        <v>86</v>
+      </c>
+      <c r="M2" t="s">
+        <v>87</v>
+      </c>
+      <c r="N2">
+        <v>89149</v>
+      </c>
+      <c r="O2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>89</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>90</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{DF074A23-F44F-48D9-87D7-5C171FE04C53}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -641,12 +1458,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8605BC2E-416F-42B3-84A2-B10816354C93}">
   <dimension ref="A1:N5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -898,7 +1715,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AD8BD9-3163-4ED5-AF75-487BD02048D4}">
   <dimension ref="A1:C17"/>
   <sheetViews>
@@ -1079,4 +1896,45 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558DEA5D-9A4A-4E7C-8517-ABB02B8C34DD}">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="61.21875" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.21875" customWidth="1"/>
+    <col min="11" max="11" width="19.77734375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="15.44140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" s="1" customFormat="1" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G2" s="2"/>
+      <c r="R2" s="4"/>
+      <c r="S2" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>